<commit_message>
Fix the issue with the spreadsheet templates admins can download.
Move the generation of the supplier data into a seperate rake task.
</commit_message>
<xml_diff>
--- a/data/facilities_management/rm6232/RM6232 Supplier Services (for Dev & Test).xlsx
+++ b/data/facilities_management/rm6232/RM6232 Supplier Services (for Dev & Test).xlsx
@@ -247,10 +247,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Supplier name</t>
+        </is>
+      </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
           <t>Abshire, Schumm and Farrell</t>
@@ -378,10 +382,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>DUNS number</t>
+        </is>
+      </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
           <t>602014337</t>
@@ -10597,7 +10605,7 @@
     <row r="92">
       <c r="A92" s="8" t="inlineStr">
         <is>
-          <t>Service N:12 - Janitor Services (Education)</t>
+          <t>Service N:12 - Janitor Services</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -13711,10 +13719,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Supplier name</t>
+        </is>
+      </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
           <t>Abshire, Schumm and Farrell</t>
@@ -13822,10 +13834,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>DUNS number</t>
+        </is>
+      </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
           <t>602014337</t>
@@ -22641,7 +22657,7 @@
     <row r="92">
       <c r="A92" s="8" t="inlineStr">
         <is>
-          <t>Service N:12 - Janitor Services (Education)</t>
+          <t>Service N:12 - Janitor Services</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -25339,10 +25355,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Supplier name</t>
+        </is>
+      </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
           <t>Berge-Koepp</t>
@@ -25470,10 +25490,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>DUNS number</t>
+        </is>
+      </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
           <t>836646194</t>
@@ -35689,7 +35713,7 @@
     <row r="92">
       <c r="A92" s="8" t="inlineStr">
         <is>
-          <t>Service N:12 - Janitor Services (Education)</t>
+          <t>Service N:12 - Janitor Services</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -38807,10 +38831,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Supplier name</t>
+        </is>
+      </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
           <t>Abshire, Schumm and Farrell</t>
@@ -38938,10 +38966,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>DUNS number</t>
+        </is>
+      </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
           <t>602014337</t>
@@ -41614,10 +41646,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Supplier name</t>
+        </is>
+      </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
           <t>Abshire, Schumm and Farrell</t>
@@ -41725,10 +41761,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>DUNS number</t>
+        </is>
+      </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
           <t>602014337</t>
@@ -44045,10 +44085,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Supplier name</t>
+        </is>
+      </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
           <t>Berge-Koepp</t>
@@ -44176,10 +44220,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>DUNS number</t>
+        </is>
+      </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
           <t>836646194</t>
@@ -46856,10 +46904,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Supplier name</t>
+        </is>
+      </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
           <t>Abshire, Schumm and Farrell</t>
@@ -46987,10 +47039,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>DUNS number</t>
+        </is>
+      </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
           <t>602014337</t>
@@ -55015,7 +55071,7 @@
     <row r="73">
       <c r="A73" s="8" t="inlineStr">
         <is>
-          <t>Service N:12 - Janitor Services (Education)</t>
+          <t>Service N:12 - Janitor Services</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -55358,10 +55414,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Supplier name</t>
+        </is>
+      </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
           <t>Abshire, Schumm and Farrell</t>
@@ -55469,10 +55529,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>DUNS number</t>
+        </is>
+      </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
           <t>602014337</t>
@@ -62397,7 +62461,7 @@
     <row r="73">
       <c r="A73" s="8" t="inlineStr">
         <is>
-          <t>Service N:12 - Janitor Services (Education)</t>
+          <t>Service N:12 - Janitor Services</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -62704,10 +62768,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Supplier name</t>
+        </is>
+      </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
           <t>Berge-Koepp</t>
@@ -62835,10 +62903,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>DUNS number</t>
+        </is>
+      </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
           <t>836646194</t>
@@ -70863,7 +70935,7 @@
     <row r="73">
       <c r="A73" s="8" t="inlineStr">
         <is>
-          <t>Service N:12 - Janitor Services (Education)</t>
+          <t>Service N:12 - Janitor Services</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">

</xml_diff>